<commit_message>
added types to costume table
</commit_message>
<xml_diff>
--- a/costumeTable.xlsx
+++ b/costumeTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>CostumeId</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>auto incremented</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>eg, character, slasher, emergency worker, monster….</t>
   </si>
 </sst>
 </file>
@@ -362,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,9 +379,10 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,13 +398,19 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>